<commit_message>
Updated version of motor board and main board
</commit_message>
<xml_diff>
--- a/CAD/electrical/motor_board_v3/bom.xlsx
+++ b/CAD/electrical/motor_board_v3/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -34,36 +34,36 @@
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
   <si>
+    <t xml:space="preserve">100n capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1,C2,C4,C6,C8,C9,C10,C14,C15,C16,C20,C21,C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10n 50V capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7,C13,C19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C57112</t>
+  </si>
+  <si>
     <t xml:space="preserve">22p capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
+    <t xml:space="preserve">C11,C17</t>
   </si>
   <si>
     <t xml:space="preserve">C1653</t>
   </si>
   <si>
-    <t xml:space="preserve">100n capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4,C6,C8,C9,C10,C11,C14,C15,C16,C17,C20,C21,C22,C23,C25,C26,C27,C28,C33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C14663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10n (50V) capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7,C13,C19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C57112</t>
-  </si>
-  <si>
     <t xml:space="preserve">470n capacitor</t>
   </si>
   <si>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">300 resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R4,R6,R7,R8</t>
+    <t xml:space="preserve">R1,R4,R6,R7</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor_SMD:R_1206_3216Metric</t>
@@ -166,15 +166,24 @@
     <t xml:space="preserve">C17887</t>
   </si>
   <si>
+    <t xml:space="preserve">220 resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2,R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22962</t>
+  </si>
+  <si>
     <t xml:space="preserve">120 resistor</t>
   </si>
   <si>
     <t xml:space="preserve">R5</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">C22787</t>
   </si>
   <si>
@@ -199,22 +208,22 @@
     <t xml:space="preserve">10k resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R18</t>
+    <t xml:space="preserve">R18,R19</t>
   </si>
   <si>
     <t xml:space="preserve">C25804</t>
   </si>
   <si>
-    <t xml:space="preserve">STM32F401RCT</t>
+    <t xml:space="preserve">Atmega328PB</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_QFP:LQFP-64_10x10mm_P0.5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C74524</t>
+    <t xml:space="preserve">Package_QFP:TQFP-32_7x7mm_P0.8mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C132230</t>
   </si>
   <si>
     <t xml:space="preserve">SN75176BDR</t>
@@ -241,22 +250,10 @@
     <t xml:space="preserve">C81582</t>
   </si>
   <si>
-    <t xml:space="preserve">AMS1117-3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6186</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRV05-4</t>
   </si>
   <si>
-    <t xml:space="preserve">U8</t>
+    <t xml:space="preserve">U8,U6</t>
   </si>
   <si>
     <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-6</t>
@@ -265,7 +262,7 @@
     <t xml:space="preserve">C85364</t>
   </si>
   <si>
-    <t xml:space="preserve">25 MHz crystal</t>
+    <t xml:space="preserve">16MHz crystal</t>
   </si>
   <si>
     <t xml:space="preserve">Y1</t>
@@ -274,7 +271,7 @@
     <t xml:space="preserve">Crystal:Crystal_SMD_3225-4Pin_3.2x2.5mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C9006</t>
+    <t xml:space="preserve">C13738</t>
   </si>
 </sst>
 </file>
@@ -382,10 +379,10 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.08"/>
@@ -431,7 +428,7 @@
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -445,7 +442,7 @@
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -575,7 +572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>48</v>
       </c>
@@ -611,7 +608,7 @@
         <v>56</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>57</v>
@@ -625,9 +622,9 @@
         <v>59</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -639,80 +636,80 @@
         <v>62</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated version of motor board and main board (#3)
* Cleaning backup files

* [WIP] Main board V2

* [WIP] Implement RS485 in ultrasonic board

* Updated version of motor board and main board
</commit_message>
<xml_diff>
--- a/CAD/electrical/motor_board_v3/bom.xlsx
+++ b/CAD/electrical/motor_board_v3/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -34,36 +34,36 @@
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
   <si>
+    <t xml:space="preserve">100n capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1,C2,C4,C6,C8,C9,C10,C14,C15,C16,C20,C21,C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14663</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10n 50V capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7,C13,C19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C57112</t>
+  </si>
+  <si>
     <t xml:space="preserve">22p capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
+    <t xml:space="preserve">C11,C17</t>
   </si>
   <si>
     <t xml:space="preserve">C1653</t>
   </si>
   <si>
-    <t xml:space="preserve">100n capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4,C6,C8,C9,C10,C11,C14,C15,C16,C17,C20,C21,C22,C23,C25,C26,C27,C28,C33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C14663</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10n (50V) capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7,C13,C19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C57112</t>
-  </si>
-  <si>
     <t xml:space="preserve">470n capacitor</t>
   </si>
   <si>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">300 resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R4,R6,R7,R8</t>
+    <t xml:space="preserve">R1,R4,R6,R7</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor_SMD:R_1206_3216Metric</t>
@@ -166,15 +166,24 @@
     <t xml:space="preserve">C17887</t>
   </si>
   <si>
+    <t xml:space="preserve">220 resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2,R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22962</t>
+  </si>
+  <si>
     <t xml:space="preserve">120 resistor</t>
   </si>
   <si>
     <t xml:space="preserve">R5</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">C22787</t>
   </si>
   <si>
@@ -199,22 +208,22 @@
     <t xml:space="preserve">10k resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R18</t>
+    <t xml:space="preserve">R18,R19</t>
   </si>
   <si>
     <t xml:space="preserve">C25804</t>
   </si>
   <si>
-    <t xml:space="preserve">STM32F401RCT</t>
+    <t xml:space="preserve">Atmega328PB</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_QFP:LQFP-64_10x10mm_P0.5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C74524</t>
+    <t xml:space="preserve">Package_QFP:TQFP-32_7x7mm_P0.8mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C132230</t>
   </si>
   <si>
     <t xml:space="preserve">SN75176BDR</t>
@@ -241,22 +250,10 @@
     <t xml:space="preserve">C81582</t>
   </si>
   <si>
-    <t xml:space="preserve">AMS1117-3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6186</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRV05-4</t>
   </si>
   <si>
-    <t xml:space="preserve">U8</t>
+    <t xml:space="preserve">U8,U6</t>
   </si>
   <si>
     <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23-6</t>
@@ -265,7 +262,7 @@
     <t xml:space="preserve">C85364</t>
   </si>
   <si>
-    <t xml:space="preserve">25 MHz crystal</t>
+    <t xml:space="preserve">16MHz crystal</t>
   </si>
   <si>
     <t xml:space="preserve">Y1</t>
@@ -274,7 +271,7 @@
     <t xml:space="preserve">Crystal:Crystal_SMD_3225-4Pin_3.2x2.5mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C9006</t>
+    <t xml:space="preserve">C13738</t>
   </si>
 </sst>
 </file>
@@ -382,10 +379,10 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.08"/>
@@ -431,7 +428,7 @@
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -445,7 +442,7 @@
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -575,7 +572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>48</v>
       </c>
@@ -611,7 +608,7 @@
         <v>56</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>57</v>
@@ -625,9 +622,9 @@
         <v>59</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -639,80 +636,80 @@
         <v>62</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="1" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>